<commit_message>
tentavivas falhas de pdf para excel formatado
</commit_message>
<xml_diff>
--- a/livro fiscal/resultado.xlsx
+++ b/livro fiscal/resultado.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,8 +48,8 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,42 +416,105 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A10:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="986" customWidth="1" min="1" max="1"/>
-  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>PREFEITURA MUNICIPAL DE ITAPIRA - SP
-Secretaria Municipal dos Negócios da Fazenda - Fiscalização Tributária
-Apuração do ISSQN - Livro Fiscal - Serviços Prestados
-CCM: CPF / CNPJ: Mês Referência: Situação: Encerramento:
-44032 18879337000186 Janeiro/2025 Mês Encerrado 30/01/2025 09:54:13
-Razão Social:
-TRIO ARENA UNIVERSITARIA LTDA.
-Endereço: Número:
-ALBANO PEGORARI 405
-Complemento: Bairro: Cidade: Estado:
-VILA PENHA DO RIO DO PEIXE ITAPIRA SP
-IP: 172.16.20.60 Data impressão: 05/02/2025 10:34:24
-LANÇAMENTOS VÁLIDOS
-Dia Número Série Tipo Situação Cod. Aliq.(%) Base(R$) ISS(R$) CNPJ Tomador Razão Tomador Lanç.
-8 99 1 Eletrônica Não Trib. 1212 2,01 5500,00 - 44.766.996/0001-16 CERAMICA CLUBE Norm.
-20 100 1 Eletrônica Não Trib. 1212 2,01 12000,00 - 71.262.273/0001-52 SERRA NEGRA ESPORTE CLUBE Norm.
-Total: 17500,00 0,00
-LANÇAMENTOS SUBSTITUÍDOS E CANCELADOS
-Dia Número Série Tipo Situação Cod. Aliq.(%) Base(R$) ISS(R$) CNPJ Tomador Razão Tomador Evento
-Sem Lançamentos no Período</t>
-        </is>
-      </c>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>CCM:</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>CPF / CNPJ:</t>
+        </is>
+      </c>
+      <c r="I10" s="1" t="inlineStr">
+        <is>
+          <t>Mês Referência:</t>
+        </is>
+      </c>
+      <c r="L10" s="1" t="inlineStr">
+        <is>
+          <t>Situação:</t>
+        </is>
+      </c>
+      <c r="O10" s="1" t="inlineStr">
+        <is>
+          <t>Encerramento:</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr"/>
+      <c r="E11" s="1" t="inlineStr"/>
+      <c r="I11" s="1" t="inlineStr"/>
+      <c r="L11" s="1" t="inlineStr"/>
+      <c r="O11" s="1" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Razão Social:</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>TRIO ARENA UNIVERSITARIA LTDA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Endereço:</t>
+        </is>
+      </c>
+      <c r="J14" s="1" t="inlineStr">
+        <is>
+          <t>Número:</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr"/>
+      <c r="J15" s="1" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Complemento:</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>Bairro:</t>
+        </is>
+      </c>
+      <c r="I16" s="1" t="inlineStr">
+        <is>
+          <t>Cidade:</t>
+        </is>
+      </c>
+      <c r="N16" s="1" t="inlineStr">
+        <is>
+          <t>Estado:</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr"/>
+      <c r="E17" s="1" t="inlineStr"/>
+      <c r="I17" s="1" t="inlineStr"/>
+      <c r="N17" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>